<commit_message>
Adjusted number of properties data collected for and resized graph window
</commit_message>
<xml_diff>
--- a/property_data.xlsx
+++ b/property_data.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="newcastle_upon_tyne_properties" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cardiff_properties" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="barry_properties" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -573,8 +575,6 @@
           <t>Quayside Stay...</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
         <v>122</v>
       </c>
@@ -993,6 +993,626 @@
       </c>
       <c r="D35" t="n">
         <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>average_rating</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_ratings</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>price_per_night</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A lovely private...</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="C2" t="n">
+        <v>7</v>
+      </c>
+      <c r="D2" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Room in Cardiff ...</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>City Centre Retr...</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="C4" t="n">
+        <v>366</v>
+      </c>
+      <c r="D4" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Warm &amp; welcoming...</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="C5" t="n">
+        <v>951</v>
+      </c>
+      <c r="D5" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cosy &amp; Central S...</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4.79</v>
+      </c>
+      <c r="C6" t="n">
+        <v>53</v>
+      </c>
+      <c r="D6" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Central &amp; Modern...</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="C7" t="n">
+        <v>84</v>
+      </c>
+      <c r="D7" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Detached, indepe...</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="C8" t="n">
+        <v>380</v>
+      </c>
+      <c r="D8" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>5 mins to Centre...</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.79</v>
+      </c>
+      <c r="C9" t="n">
+        <v>192</v>
+      </c>
+      <c r="D9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Single room in g...</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="C10" t="n">
+        <v>329</v>
+      </c>
+      <c r="D10" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Central &amp; Modern...</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4.89</v>
+      </c>
+      <c r="C11" t="n">
+        <v>94</v>
+      </c>
+      <c r="D11" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>The Little Lake ...</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="C12" t="n">
+        <v>739</v>
+      </c>
+      <c r="D12" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Spacious Detache...</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="C13" t="n">
+        <v>202</v>
+      </c>
+      <c r="D13" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Cosy Victorian h...</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C14" t="n">
+        <v>236</v>
+      </c>
+      <c r="D14" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Cosy cabin style...</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="C15" t="n">
+        <v>505</v>
+      </c>
+      <c r="D15" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Double Room / Ow...</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="C16" t="n">
+        <v>543</v>
+      </c>
+      <c r="D16" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Compact Tiny Taf...</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="C17" t="n">
+        <v>170</v>
+      </c>
+      <c r="D17" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>(B) Private En-s...</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="C18" t="n">
+        <v>284</v>
+      </c>
+      <c r="D18" t="n">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>average_rating</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_ratings</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>price_per_night</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>The Annex @ Broo...</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="C2" t="n">
+        <v>153</v>
+      </c>
+      <c r="D2" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>"Y Sied"-quiet, ...</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="C3" t="n">
+        <v>206</v>
+      </c>
+      <c r="D3" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Double bed w/ en...</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="C4" t="n">
+        <v>64</v>
+      </c>
+      <c r="D4" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Comfy small room...</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4.71</v>
+      </c>
+      <c r="C5" t="n">
+        <v>340</v>
+      </c>
+      <c r="D5" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Crow's Nest Barr...</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="C6" t="n">
+        <v>51</v>
+      </c>
+      <c r="D6" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Cosy Gladstone...</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.72</v>
+      </c>
+      <c r="C7" t="n">
+        <v>250</v>
+      </c>
+      <c r="D7" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sea view, entire...</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="C8" t="n">
+        <v>64</v>
+      </c>
+      <c r="D8" t="n">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Lovely light sum...</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="C9" t="n">
+        <v>145</v>
+      </c>
+      <c r="D9" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Bright Seaside H...</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="C10" t="n">
+        <v>212</v>
+      </c>
+      <c r="D10" t="n">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Vale View (Barry...</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="C11" t="n">
+        <v>29</v>
+      </c>
+      <c r="D11" t="n">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Detached house o...</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>6</v>
+      </c>
+      <c r="D12" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>The 19th Dock...</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>9</v>
+      </c>
+      <c r="D13" t="n">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>luxury 2 bedroom...</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="C14" t="n">
+        <v>83</v>
+      </c>
+      <c r="D14" t="n">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>The Little Blue ...</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8</v>
+      </c>
+      <c r="D15" t="n">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Large detached h...</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C16" t="n">
+        <v>49</v>
+      </c>
+      <c r="D16" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Room - Garden Vi...</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Ty Hapus is a 3-...</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="C18" t="n">
+        <v>193</v>
+      </c>
+      <c r="D18" t="n">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create GUI Adds a functional GUI for the user that takes their input using labels an entry and a button
</commit_message>
<xml_diff>
--- a/property_data.xlsx
+++ b/property_data.xlsx
@@ -10,6 +10,10 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="newcastle_upon_tyne_properties" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cardiff_properties" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="barry_properties" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Devon_properties" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bristol_properties" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="birmingham_properties" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="new_york_properties" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1618,4 +1622,1230 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>average_rating</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_ratings</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>price_per_night</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>No Snakes on thi...</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Exceptionally be...</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>53</v>
+      </c>
+      <c r="D3" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Tranquil Room by...</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>12</v>
+      </c>
+      <c r="D4" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cosy barn betwee...</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>The Cabin Devon ...</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>409</v>
+      </c>
+      <c r="D6" t="n">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>The Cabin at Axe...</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="C7" t="n">
+        <v>150</v>
+      </c>
+      <c r="D7" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Hattie - luxury ...</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="C8" t="n">
+        <v>72</v>
+      </c>
+      <c r="D8" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Swaledale Shephe...</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="C9" t="n">
+        <v>198</v>
+      </c>
+      <c r="D9" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Cosy Idyllic Cab...</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="C10" t="n">
+        <v>551</v>
+      </c>
+      <c r="D10" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Lakeside Lodge, ...</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>119</v>
+      </c>
+      <c r="D11" t="n">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>The Wizards Caul...</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>165</v>
+      </c>
+      <c r="D12" t="n">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Luxury Roundhous...</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="C13" t="n">
+        <v>38</v>
+      </c>
+      <c r="D13" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Outstanding self...</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>381</v>
+      </c>
+      <c r="D14" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Cosy traditional...</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>5</v>
+      </c>
+      <c r="C15" t="n">
+        <v>6</v>
+      </c>
+      <c r="D15" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Luxury Shepherds...</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>5</v>
+      </c>
+      <c r="C16" t="n">
+        <v>130</v>
+      </c>
+      <c r="D16" t="n">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>The Shippon. Uni...</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="C17" t="n">
+        <v>331</v>
+      </c>
+      <c r="D17" t="n">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ModburyLittleHom...</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4.84</v>
+      </c>
+      <c r="C18" t="n">
+        <v>133</v>
+      </c>
+      <c r="D18" t="n">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>average_rating</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_ratings</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>price_per_night</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Modern Comfort C...</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>30</v>
+      </c>
+      <c r="D2" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>The Great Room N...</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="C3" t="n">
+        <v>94</v>
+      </c>
+      <c r="D3" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Toad Lodge The B...</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4.83</v>
+      </c>
+      <c r="C4" t="n">
+        <v>345</v>
+      </c>
+      <c r="D4" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Comfortable, cos...</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>12</v>
+      </c>
+      <c r="D5" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Entire home in E...</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Twin room in fam...</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="C7" t="n">
+        <v>130</v>
+      </c>
+      <c r="D7" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Clifton cosy bed...</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4.78</v>
+      </c>
+      <c r="C8" t="n">
+        <v>181</v>
+      </c>
+      <c r="D8" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Comfortable room...</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="C9" t="n">
+        <v>166</v>
+      </c>
+      <c r="D9" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Spacious Double ...</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="C10" t="n">
+        <v>21</v>
+      </c>
+      <c r="D10" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Cosy boutique ci...</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>13</v>
+      </c>
+      <c r="D11" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Perfectly Locate...</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>6</v>
+      </c>
+      <c r="D12" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Tuscany House...</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="C13" t="n">
+        <v>45</v>
+      </c>
+      <c r="D13" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Palm House an ur...</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>29</v>
+      </c>
+      <c r="D14" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>The Robinson Bui...</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.93</v>
+      </c>
+      <c r="C15" t="n">
+        <v>135</v>
+      </c>
+      <c r="D15" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Private self con...</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="C16" t="n">
+        <v>145</v>
+      </c>
+      <c r="D16" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Riverside Walk...</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="C17" t="n">
+        <v>213</v>
+      </c>
+      <c r="D17" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Self contained a...</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="C18" t="n">
+        <v>141</v>
+      </c>
+      <c r="D18" t="n">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>average_rating</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_ratings</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>price_per_night</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Plough House - 5...</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>210</v>
+      </c>
+      <c r="D2" t="n">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Double room with...</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1 Bed Flat, with...</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Comfy NEC/Airpor...</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kula Birmingham ...</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4.81</v>
+      </c>
+      <c r="C6" t="n">
+        <v>113</v>
+      </c>
+      <c r="D6" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Double Room2 wit...</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="C7" t="n">
+        <v>253</v>
+      </c>
+      <c r="D7" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Cozy Stay Near A...</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4.83</v>
+      </c>
+      <c r="C8" t="n">
+        <v>46</v>
+      </c>
+      <c r="D8" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>The Foxes Den - ...</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="C9" t="n">
+        <v>620</v>
+      </c>
+      <c r="D9" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>'Heron's Rest' c...</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="C10" t="n">
+        <v>162</v>
+      </c>
+      <c r="D10" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Lovely Room by U...</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Unique chalet ho...</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="C12" t="n">
+        <v>363</v>
+      </c>
+      <c r="D12" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2 Bed Flat - Cen...</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Cosy 1 bedroom e...</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="C14" t="n">
+        <v>28</v>
+      </c>
+      <c r="D14" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>The Blue Room...</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8</v>
+      </c>
+      <c r="D15" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Studio Near HS2,...</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Room in West Mid...</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4.93</v>
+      </c>
+      <c r="C17" t="n">
+        <v>14</v>
+      </c>
+      <c r="D17" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Bed 10m from Bir...</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C18" t="n">
+        <v>81</v>
+      </c>
+      <c r="D18" t="n">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>average_rating</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_ratings</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>price_per_night</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Home from home &amp;...</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>19</v>
+      </c>
+      <c r="D2" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>3 BD | Luxury St...</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Holywell Grange ...</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="C4" t="n">
+        <v>162</v>
+      </c>
+      <c r="D4" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Home from home,b...</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="C5" t="n">
+        <v>166</v>
+      </c>
+      <c r="D5" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>3 bed house in S...</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>A single room 20...</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="C7" t="n">
+        <v>108</v>
+      </c>
+      <c r="D7" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1 Bedroom House ...</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>135</v>
+      </c>
+      <c r="D8" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Stylish 3 bed ho...</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="C9" t="n">
+        <v>77</v>
+      </c>
+      <c r="D9" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Comfortable sing...</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>13</v>
+      </c>
+      <c r="D10" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Seghill’s Sanctu...</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4.89</v>
+      </c>
+      <c r="C11" t="n">
+        <v>123</v>
+      </c>
+      <c r="D11" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>RestfullStays- S...</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4.64</v>
+      </c>
+      <c r="C12" t="n">
+        <v>33</v>
+      </c>
+      <c r="D12" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Stylish and Cosy...</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Tiny Homestead@W...</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="C14" t="n">
+        <v>212</v>
+      </c>
+      <c r="D14" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>House in Westmoo...</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="C15" t="n">
+        <v>42</v>
+      </c>
+      <c r="D15" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>THE PLUMES Heato...</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="C16" t="n">
+        <v>285</v>
+      </c>
+      <c r="D16" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Studio in leafy ...</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="C17" t="n">
+        <v>485</v>
+      </c>
+      <c r="D17" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Lovely bright si...</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="C18" t="n">
+        <v>167</v>
+      </c>
+      <c r="D18" t="n">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
a few final tweaks
</commit_message>
<xml_diff>
--- a/property_data.xlsx
+++ b/property_data.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="4" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="newcastle_upon_tyne_properties" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,22 +13,33 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bristol_properties" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="birmingham_properties" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="new_york_properties" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dorchester_properties" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bournemouth_properties" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Poole_properties" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Milton_Keynes_properties" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MIlton_Keynes_properties1" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -43,12 +53,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -61,14 +86,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -437,25 +465,911 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>average_rating</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_ratings</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>price_per_night</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>HNFC Stays - Uni...</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4.78</v>
+      </c>
+      <c r="C2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D2" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Small Double Roo...</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="C3" t="n">
+        <v>97</v>
+      </c>
+      <c r="D3" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Studio in leafy ...</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="C4" t="n">
+        <v>485</v>
+      </c>
+      <c r="D4" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Double room + Ne...</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="C5" t="n">
+        <v>70</v>
+      </c>
+      <c r="D5" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Adonia Apartment...</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="C6" t="n">
+        <v>254</v>
+      </c>
+      <c r="D6" t="n">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>The Gosforth Ret...</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="C7" t="n">
+        <v>151</v>
+      </c>
+      <c r="D7" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Friendly family ...</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Quayside Stay...</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>House near Hadri...</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="C10" t="n">
+        <v>261</v>
+      </c>
+      <c r="D10" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Luxurious &amp; Spac...</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>12</v>
+      </c>
+      <c r="D11" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Ensuite Room in ...</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="C12" t="n">
+        <v>15</v>
+      </c>
+      <c r="D12" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Cosy Escape by H...</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>18</v>
+      </c>
+      <c r="D13" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Cosy Double Room...</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>4.89</v>
+      </c>
+      <c r="C14" t="n">
+        <v>55</v>
+      </c>
+      <c r="D14" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Elegant city apa...</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="C15" t="n">
+        <v>61</v>
+      </c>
+      <c r="D15" t="n">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Stunning Central...</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="C16" t="n">
+        <v>445</v>
+      </c>
+      <c r="D16" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Historic City Ce...</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>59</v>
+      </c>
+      <c r="D17" t="n">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>High Quay...</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="C18" t="n">
+        <v>124</v>
+      </c>
+      <c r="D18" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1 Bedroom House ...</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>135</v>
+      </c>
+      <c r="D19" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Cozy Seaview Roo...</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>8</v>
+      </c>
+      <c r="D20" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Cosy double bedr...</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>4.93</v>
+      </c>
+      <c r="C21" t="n">
+        <v>112</v>
+      </c>
+      <c r="D21" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>HNFC Stays - Exc...</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>4.93</v>
+      </c>
+      <c r="C22" t="n">
+        <v>14</v>
+      </c>
+      <c r="D22" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>****NO CLEANING ...</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>4.81</v>
+      </c>
+      <c r="C23" t="n">
+        <v>486</v>
+      </c>
+      <c r="D23" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Home from home,b...</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="C24" t="n">
+        <v>166</v>
+      </c>
+      <c r="D24" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Quirky Self cont...</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C25" t="n">
+        <v>730</v>
+      </c>
+      <c r="D25" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Spacious 3-br Ho...</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>5</v>
+      </c>
+      <c r="C26" t="n">
+        <v>7</v>
+      </c>
+      <c r="D26" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Modern, Minimali...</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="C27" t="n">
+        <v>34</v>
+      </c>
+      <c r="D27" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Churchill Street...</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>5</v>
+      </c>
+      <c r="C28" t="n">
+        <v>20</v>
+      </c>
+      <c r="D28" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>EnquireNow - Big...</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>5</v>
+      </c>
+      <c r="C29" t="n">
+        <v>4</v>
+      </c>
+      <c r="D29" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>THE PLUMES Heato...</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="C30" t="n">
+        <v>285</v>
+      </c>
+      <c r="D30" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Studio Apartment...</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="C31" t="n">
+        <v>126</v>
+      </c>
+      <c r="D31" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>A single room 20...</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="C32" t="n">
+        <v>108</v>
+      </c>
+      <c r="D32" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Large Private Ro...</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>4.81</v>
+      </c>
+      <c r="C33" t="n">
+        <v>48</v>
+      </c>
+      <c r="D33" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Pool Table House...</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>City Villa Apart...</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>4.49</v>
+      </c>
+      <c r="C35" t="n">
+        <v>65</v>
+      </c>
+      <c r="D35" t="n">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>average_rating</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_ratings</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>price_per_night</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Private Studio G...</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="C2" t="n">
+        <v>238</v>
+      </c>
+      <c r="D2" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>The Little Cabin...</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4.93</v>
+      </c>
+      <c r="C3" t="n">
+        <v>516</v>
+      </c>
+      <c r="D3" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>The Studio ( Pri...</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4.93</v>
+      </c>
+      <c r="C4" t="n">
+        <v>107</v>
+      </c>
+      <c r="D4" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>The Retreat...</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>14</v>
+      </c>
+      <c r="D5" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Single room in q...</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="C6" t="n">
+        <v>106</v>
+      </c>
+      <c r="D6" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Spacious single ...</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>63</v>
+      </c>
+      <c r="D7" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Exquisite Holida...</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="C8" t="n">
+        <v>244</v>
+      </c>
+      <c r="D8" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Double Bedroom w...</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="C9" t="n">
+        <v>104</v>
+      </c>
+      <c r="D9" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Cheerful small p...</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="C10" t="n">
+        <v>157</v>
+      </c>
+      <c r="D10" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Cosy Studio Apar...</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>A cozy town cent...</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="C12" t="n">
+        <v>13</v>
+      </c>
+      <c r="D12" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Single bedroom i...</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="C13" t="n">
+        <v>7</v>
+      </c>
+      <c r="D13" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>6 mins drive to ...</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="C14" t="n">
+        <v>202</v>
+      </c>
+      <c r="D14" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Large Stylish fl...</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>5</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>The Cabin - Hot ...</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="C16" t="n">
+        <v>544</v>
+      </c>
+      <c r="D16" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Up in the clouds...</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4.76</v>
+      </c>
+      <c r="C17" t="n">
+        <v>134</v>
+      </c>
+      <c r="D17" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Warm and Cosy Ca...</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>10</v>
+      </c>
+      <c r="D18" t="n">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>average_rating</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>number_of_ratings</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>price_per_night</t>
         </is>
@@ -464,103 +1378,400 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HNFC Stays - Uni...</t>
+          <t>A tranquil oasis...</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.78</v>
+        <v>4.97</v>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>714</v>
       </c>
       <c r="D2" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Small Double Roo...</t>
+          <t>Willen - guest s...</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.82</v>
+        <v>4.98</v>
       </c>
       <c r="C3" t="n">
-        <v>97</v>
+        <v>199</v>
       </c>
       <c r="D3" t="n">
-        <v>29</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Studio in leafy ...</t>
+          <t># 2 Luxury apart...</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4.98</v>
+        <v>4.89</v>
       </c>
       <c r="C4" t="n">
-        <v>485</v>
+        <v>53</v>
       </c>
       <c r="D4" t="n">
-        <v>67</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Double room + Ne...</t>
+          <t>Live music fan? ...</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.99</v>
+        <v>4.57</v>
       </c>
       <c r="C5" t="n">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Adonia Apartment...</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>4.95</v>
-      </c>
-      <c r="C6" t="n">
-        <v>254</v>
+          <t>Apartment in Cen...</t>
+        </is>
       </c>
       <c r="D6" t="n">
-        <v>156</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>The Gosforth Ret...</t>
+          <t>single room clos...</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.92</v>
+        <v>4.87</v>
       </c>
       <c r="C7" t="n">
-        <v>151</v>
+        <v>82</v>
       </c>
       <c r="D7" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Friendly family ...</t>
+          <t>En-suite private...</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="C8" t="n">
+        <v>95</v>
+      </c>
+      <c r="D8" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Single Room | Sm...</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="C9" t="n">
+        <v>66</v>
+      </c>
+      <c r="D9" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Separate Self co...</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="C10" t="n">
+        <v>117</v>
+      </c>
+      <c r="D10" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Stylish watersid...</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4.89</v>
+      </c>
+      <c r="C11" t="n">
+        <v>54</v>
+      </c>
+      <c r="D11" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>A Cosy Self-Cont...</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="C12" t="n">
+        <v>104</v>
+      </c>
+      <c r="D12" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Bright &amp; cozy cl...</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Quiet Home in Mi...</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="C14" t="n">
+        <v>35</v>
+      </c>
+      <c r="D14" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>#31 Silbury 2min...</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Double room with...</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Green! A room of...</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>7</v>
+      </c>
+      <c r="D17" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Holly Tree Hidea...</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="C18" t="n">
+        <v>63</v>
+      </c>
+      <c r="D18" t="n">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>average_rating</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>number_of_ratings</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>price_per_night</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t># 2 Luxury apart...</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4.89</v>
+      </c>
+      <c r="C2" t="n">
+        <v>53</v>
+      </c>
+      <c r="D2" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Live music fan? ...</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4.57</v>
+      </c>
+      <c r="C3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>single room clos...</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="C4" t="n">
+        <v>82</v>
+      </c>
+      <c r="D4" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>#6 Milburn,CMK l...</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>A tranquil oasis...</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="C6" t="n">
+        <v>714</v>
+      </c>
+      <c r="D6" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Private annexe w...</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Green! A room of...</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,433 +1781,159 @@
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Quayside Stay...</t>
-        </is>
+          <t>Cosy Double Room...</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.93</v>
+      </c>
+      <c r="C9" t="n">
+        <v>15</v>
       </c>
       <c r="D9" t="n">
-        <v>122</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>House near Hadri...</t>
+          <t>Stylish watersid...</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4.98</v>
+        <v>4.9</v>
       </c>
       <c r="C10" t="n">
-        <v>261</v>
+        <v>31</v>
       </c>
       <c r="D10" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Luxurious &amp; Spac...</t>
+          <t>Single Room | Sm...</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>4.95</v>
       </c>
       <c r="C11" t="n">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="D11" t="n">
-        <v>106</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ensuite Room in ...</t>
+          <t>Lovely Home Near...</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4.53</v>
+        <v>4.86</v>
       </c>
       <c r="C12" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
-        <v>34</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Cosy Escape by H...</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>5</v>
-      </c>
-      <c r="C13" t="n">
-        <v>18</v>
-      </c>
+          <t>#31 Silbury 2min...</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
-        <v>72</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Cosy Double Room...</t>
+          <t>Willen - guest s...</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4.89</v>
+        <v>4.98</v>
       </c>
       <c r="C14" t="n">
-        <v>55</v>
+        <v>199</v>
       </c>
       <c r="D14" t="n">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Elegant city apa...</t>
+          <t>Relax in a Brigh...</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4.97</v>
+        <v>4.93</v>
       </c>
       <c r="C15" t="n">
-        <v>61</v>
+        <v>266</v>
       </c>
       <c r="D15" t="n">
-        <v>124</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Stunning Central...</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>4.96</v>
-      </c>
-      <c r="C16" t="n">
-        <v>445</v>
-      </c>
+          <t>Cozy Private Roo...</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
-        <v>100</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Historic City Ce...</t>
+          <t>Stylish Central ...</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>5</v>
+        <v>4.92</v>
       </c>
       <c r="C17" t="n">
-        <v>59</v>
+        <v>300</v>
       </c>
       <c r="D17" t="n">
-        <v>141</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>High Quay...</t>
+          <t>Single room in q...</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4.94</v>
+        <v>4.75</v>
       </c>
       <c r="C18" t="n">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="D18" t="n">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>1 Bedroom House ...</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>5</v>
-      </c>
-      <c r="C19" t="n">
-        <v>135</v>
-      </c>
-      <c r="D19" t="n">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Cozy Seaview Roo...</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>5</v>
-      </c>
-      <c r="C20" t="n">
-        <v>8</v>
-      </c>
-      <c r="D20" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Cosy double bedr...</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>4.93</v>
-      </c>
-      <c r="C21" t="n">
-        <v>112</v>
-      </c>
-      <c r="D21" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>HNFC Stays - Exc...</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>4.93</v>
-      </c>
-      <c r="C22" t="n">
-        <v>14</v>
-      </c>
-      <c r="D22" t="n">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>****NO CLEANING ...</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>4.81</v>
-      </c>
-      <c r="C23" t="n">
-        <v>486</v>
-      </c>
-      <c r="D23" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Home from home,b...</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>4.86</v>
-      </c>
-      <c r="C24" t="n">
-        <v>166</v>
-      </c>
-      <c r="D24" t="n">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Quirky Self cont...</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="C25" t="n">
-        <v>730</v>
-      </c>
-      <c r="D25" t="n">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Spacious 3-br Ho...</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>5</v>
-      </c>
-      <c r="C26" t="n">
-        <v>7</v>
-      </c>
-      <c r="D26" t="n">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Modern, Minimali...</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>4.41</v>
-      </c>
-      <c r="C27" t="n">
-        <v>34</v>
-      </c>
-      <c r="D27" t="n">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Churchill Street...</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>5</v>
-      </c>
-      <c r="C28" t="n">
-        <v>20</v>
-      </c>
-      <c r="D28" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>EnquireNow - Big...</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>5</v>
-      </c>
-      <c r="C29" t="n">
-        <v>4</v>
-      </c>
-      <c r="D29" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>THE PLUMES Heato...</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>4.96</v>
-      </c>
-      <c r="C30" t="n">
-        <v>285</v>
-      </c>
-      <c r="D30" t="n">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Studio Apartment...</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>4.98</v>
-      </c>
-      <c r="C31" t="n">
-        <v>126</v>
-      </c>
-      <c r="D31" t="n">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>A single room 20...</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>4.91</v>
-      </c>
-      <c r="C32" t="n">
-        <v>108</v>
-      </c>
-      <c r="D32" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Large Private Ro...</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>4.81</v>
-      </c>
-      <c r="C33" t="n">
-        <v>48</v>
-      </c>
-      <c r="D33" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Pool Table House...</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>0</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" t="n">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>City Villa Apart...</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>4.49</v>
-      </c>
-      <c r="C35" t="n">
-        <v>65</v>
-      </c>
-      <c r="D35" t="n">
-        <v>83</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1016,7 +1953,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1323,7 +2260,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1636,7 +2573,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1949,7 +2886,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -2256,7 +3193,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -2557,7 +3494,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -2603,8 +3540,6 @@
           <t>3 BD | Luxury St...</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
         <v>95</v>
       </c>
@@ -2647,8 +3582,6 @@
           <t>3 bed house in S...</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
         <v>136</v>
       </c>
@@ -2843,6 +3776,632 @@
       </c>
       <c r="D18" t="n">
         <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="13.33203125" customWidth="1" min="1" max="1"/>
+    <col width="9" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="9.33203125" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>average_rating</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_ratings</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>price_per_night</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Joys Nature Tent...</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Studio with off-...</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="C3" t="n">
+        <v>54</v>
+      </c>
+      <c r="D3" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>The Siding, Dorc...</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="C4" t="n">
+        <v>26</v>
+      </c>
+      <c r="D4" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Discover Little ...</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="C5" t="n">
+        <v>218</v>
+      </c>
+      <c r="D5" t="n">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Comfy double en ...</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="C6" t="n">
+        <v>187</v>
+      </c>
+      <c r="D6" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Light and airy l...</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>124</v>
+      </c>
+      <c r="D7" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>The Garden Retre...</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="C8" t="n">
+        <v>102</v>
+      </c>
+      <c r="D8" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Cheerful one bed...</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="C9" t="n">
+        <v>125</v>
+      </c>
+      <c r="D9" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Large 2 bedroom ...</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="C10" t="n">
+        <v>77</v>
+      </c>
+      <c r="D10" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Lovely, Quiet St...</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="C11" t="n">
+        <v>317</v>
+      </c>
+      <c r="D11" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Town centre room...</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Book just one or...</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="C13" t="n">
+        <v>56</v>
+      </c>
+      <c r="D13" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Walk to Town! Fr...</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="C14" t="n">
+        <v>125</v>
+      </c>
+      <c r="D14" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Room in Dorchest...</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="C15" t="n">
+        <v>46</v>
+      </c>
+      <c r="D15" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>The Attic - Bed ...</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="C16" t="n">
+        <v>50</v>
+      </c>
+      <c r="D16" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Nice n Cosy doub...</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="C17" t="n">
+        <v>52</v>
+      </c>
+      <c r="D17" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Spacious Joys do...</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="C18" t="n">
+        <v>34</v>
+      </c>
+      <c r="D18" t="n">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>average_rating</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_ratings</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>price_per_night</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2 Double bedroom...</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C2" t="n">
+        <v>29</v>
+      </c>
+      <c r="D2" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Single room Alum...</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>294</v>
+      </c>
+      <c r="D3" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cliff Heights Ap...</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cliff Manor Apt ...</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="C5" t="n">
+        <v>7</v>
+      </c>
+      <c r="D5" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>The Chess Suite ...</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8</v>
+      </c>
+      <c r="D6" t="n">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2 mins to Beach ...</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="C7" t="n">
+        <v>13</v>
+      </c>
+      <c r="D7" t="n">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Near beach with ...</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="C8" t="n">
+        <v>204</v>
+      </c>
+      <c r="D8" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>The Jumanji Suit...</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>The Beach Hytte ...</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="C10" t="n">
+        <v>137</v>
+      </c>
+      <c r="D10" t="n">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>A Hidden Gem Wit...</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="C11" t="n">
+        <v>497</v>
+      </c>
+      <c r="D11" t="n">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Beyond - Romanti...</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="C12" t="n">
+        <v>74</v>
+      </c>
+      <c r="D12" t="n">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Beach 3 Mins Wal...</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="C13" t="n">
+        <v>420</v>
+      </c>
+      <c r="D13" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>The Garden Retre...</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="C14" t="n">
+        <v>267</v>
+      </c>
+      <c r="D14" t="n">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Cosy retreat for...</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="C15" t="n">
+        <v>79</v>
+      </c>
+      <c r="D15" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Secluded garden ...</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C16" t="n">
+        <v>459</v>
+      </c>
+      <c r="D16" t="n">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Luxe Chic Retrea...</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4.64</v>
+      </c>
+      <c r="C17" t="n">
+        <v>11</v>
+      </c>
+      <c r="D17" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Log Cabin wth Ho...</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="C18" t="n">
+        <v>233</v>
+      </c>
+      <c r="D18" t="n">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removal of redundant code
</commit_message>
<xml_diff>
--- a/property_data.xlsx
+++ b/property_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="4" activeTab="7" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="8" activeTab="9" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="newcastle_upon_tyne_properties" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bournemouth_properties" sheetId="9" state="visible" r:id="rId9"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Poole_properties" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Milton_Keynes_properties" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MIlton_Keynes_properties1" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -459,31 +458,31 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>average_rating</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>number_of_ratings</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>price_per_night</t>
         </is>
@@ -492,539 +491,273 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HNFC Stays - Uni...</t>
+          <t>Friendly family ...</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.78</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Small Double Roo...</t>
+          <t>Studio in leafy ...</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.82</v>
+        <v>4.98</v>
       </c>
       <c r="C3" t="n">
-        <v>97</v>
+        <v>487</v>
       </c>
       <c r="D3" t="n">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Studio in leafy ...</t>
+          <t>The Gosforth Ret...</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4.98</v>
+        <v>4.92</v>
       </c>
       <c r="C4" t="n">
-        <v>485</v>
+        <v>152</v>
       </c>
       <c r="D4" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Double room + Ne...</t>
+          <t>Quirky Self cont...</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.99</v>
+        <v>4.9</v>
       </c>
       <c r="C5" t="n">
-        <v>70</v>
+        <v>734</v>
       </c>
       <c r="D5" t="n">
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Adonia Apartment...</t>
+          <t>Home from home,b...</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.95</v>
+        <v>4.86</v>
       </c>
       <c r="C6" t="n">
-        <v>254</v>
+        <v>167</v>
       </c>
       <c r="D6" t="n">
-        <v>156</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>The Gosforth Ret...</t>
+          <t>Walk to the worl...</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.92</v>
+        <v>4.45</v>
       </c>
       <c r="C7" t="n">
-        <v>151</v>
+        <v>96</v>
       </c>
       <c r="D7" t="n">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Friendly family ...</t>
+          <t>HNFC Stays - Bus...</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>4.83</v>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D8" t="n">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Quayside Stay...</t>
-        </is>
+          <t>Cosy en-suite ro...</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="C9" t="n">
+        <v>95</v>
       </c>
       <c r="D9" t="n">
-        <v>122</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>House near Hadri...</t>
+          <t>Elegant city apa...</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4.98</v>
+        <v>4.97</v>
       </c>
       <c r="C10" t="n">
-        <v>261</v>
+        <v>61</v>
       </c>
       <c r="D10" t="n">
-        <v>90</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Luxurious &amp; Spac...</t>
+          <t>Large bedroom in...</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D11" t="n">
-        <v>106</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ensuite Room in ...</t>
+          <t>House near Hadri...</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4.53</v>
+        <v>4.98</v>
       </c>
       <c r="C12" t="n">
-        <v>15</v>
+        <v>262</v>
       </c>
       <c r="D12" t="n">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Cosy Escape by H...</t>
+          <t>THE PLUMES Heato...</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5</v>
+        <v>4.96</v>
       </c>
       <c r="C13" t="n">
-        <v>18</v>
+        <v>286</v>
       </c>
       <c r="D13" t="n">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Cosy Double Room...</t>
+          <t>Cosy flat in Wes...</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4.89</v>
+        <v>4.93</v>
       </c>
       <c r="C14" t="n">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D14" t="n">
-        <v>41</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Elegant city apa...</t>
+          <t>Adonia Apartment...</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4.97</v>
+        <v>4.95</v>
       </c>
       <c r="C15" t="n">
-        <v>61</v>
+        <v>258</v>
       </c>
       <c r="D15" t="n">
-        <v>124</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Stunning Central...</t>
+          <t>1 Bedroom House ...</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4.96</v>
+        <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>445</v>
+        <v>136</v>
       </c>
       <c r="D16" t="n">
-        <v>100</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Historic City Ce...</t>
+          <t>Cosy Double Room...</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>5</v>
+        <v>4.89</v>
       </c>
       <c r="C17" t="n">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D17" t="n">
-        <v>141</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>High Quay...</t>
+          <t>Double room + Ne...</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4.94</v>
+        <v>4.99</v>
       </c>
       <c r="C18" t="n">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="D18" t="n">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>1 Bedroom House ...</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>5</v>
-      </c>
-      <c r="C19" t="n">
-        <v>135</v>
-      </c>
-      <c r="D19" t="n">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Cozy Seaview Roo...</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>5</v>
-      </c>
-      <c r="C20" t="n">
-        <v>8</v>
-      </c>
-      <c r="D20" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Cosy double bedr...</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>4.93</v>
-      </c>
-      <c r="C21" t="n">
-        <v>112</v>
-      </c>
-      <c r="D21" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>HNFC Stays - Exc...</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>4.93</v>
-      </c>
-      <c r="C22" t="n">
-        <v>14</v>
-      </c>
-      <c r="D22" t="n">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>****NO CLEANING ...</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>4.81</v>
-      </c>
-      <c r="C23" t="n">
-        <v>486</v>
-      </c>
-      <c r="D23" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Home from home,b...</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>4.86</v>
-      </c>
-      <c r="C24" t="n">
-        <v>166</v>
-      </c>
-      <c r="D24" t="n">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Quirky Self cont...</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="C25" t="n">
-        <v>730</v>
-      </c>
-      <c r="D25" t="n">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Spacious 3-br Ho...</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>5</v>
-      </c>
-      <c r="C26" t="n">
-        <v>7</v>
-      </c>
-      <c r="D26" t="n">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Modern, Minimali...</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>4.41</v>
-      </c>
-      <c r="C27" t="n">
-        <v>34</v>
-      </c>
-      <c r="D27" t="n">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Churchill Street...</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>5</v>
-      </c>
-      <c r="C28" t="n">
-        <v>20</v>
-      </c>
-      <c r="D28" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>EnquireNow - Big...</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>5</v>
-      </c>
-      <c r="C29" t="n">
-        <v>4</v>
-      </c>
-      <c r="D29" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>THE PLUMES Heato...</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>4.96</v>
-      </c>
-      <c r="C30" t="n">
-        <v>285</v>
-      </c>
-      <c r="D30" t="n">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Studio Apartment...</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>4.98</v>
-      </c>
-      <c r="C31" t="n">
-        <v>126</v>
-      </c>
-      <c r="D31" t="n">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>A single room 20...</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>4.91</v>
-      </c>
-      <c r="C32" t="n">
-        <v>108</v>
-      </c>
-      <c r="D32" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Large Private Ro...</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>4.81</v>
-      </c>
-      <c r="C33" t="n">
-        <v>48</v>
-      </c>
-      <c r="D33" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Pool Table House...</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>0</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" t="n">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>City Villa Apart...</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>4.49</v>
-      </c>
-      <c r="C35" t="n">
-        <v>65</v>
-      </c>
-      <c r="D35" t="n">
-        <v>83</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1040,7 +773,7 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1394,59 +1127,65 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Willen - guest s...</t>
+          <t>Private annexe w...</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.98</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>199</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>57</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t># 2 Luxury apart...</t>
+          <t>Willen - guest s...</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4.89</v>
+        <v>4.98</v>
       </c>
       <c r="C4" t="n">
-        <v>53</v>
+        <v>199</v>
       </c>
       <c r="D4" t="n">
-        <v>86</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Live music fan? ...</t>
+          <t># 2 Luxury apart...</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.57</v>
+        <v>4.89</v>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D5" t="n">
-        <v>43</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Apartment in Cen...</t>
-        </is>
+          <t>Live music fan? ...</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4.57</v>
+      </c>
+      <c r="C6" t="n">
+        <v>7</v>
       </c>
       <c r="D6" t="n">
-        <v>89</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7">
@@ -1468,123 +1207,125 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>En-suite private...</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>4.88</v>
-      </c>
-      <c r="C8" t="n">
-        <v>95</v>
-      </c>
+          <t>Apartment in Cen...</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>51</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Single Room | Sm...</t>
+          <t>En-suite private...</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>4.95</v>
+        <v>4.88</v>
       </c>
       <c r="C9" t="n">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="D9" t="n">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Separate Self co...</t>
+          <t>Single Room | Sm...</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4.96</v>
+        <v>4.95</v>
       </c>
       <c r="C10" t="n">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="D10" t="n">
-        <v>76</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Stylish watersid...</t>
+          <t>Separate Self co...</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4.89</v>
+        <v>4.96</v>
       </c>
       <c r="C11" t="n">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="D11" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>A Cosy Self-Cont...</t>
+          <t>Stylish watersid...</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4.94</v>
+        <v>4.89</v>
       </c>
       <c r="C12" t="n">
-        <v>104</v>
+        <v>54</v>
       </c>
       <c r="D12" t="n">
-        <v>74</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Bright &amp; cozy cl...</t>
+          <t>A Cosy Self-Cont...</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5</v>
+        <v>4.94</v>
       </c>
       <c r="C13" t="n">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="D13" t="n">
-        <v>36</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Quiet Home in Mi...</t>
+          <t>Bright &amp; cozy cl...</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4.97</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="D14" t="n">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>#31 Silbury 2min...</t>
-        </is>
+          <t>Quiet Home in Mi...</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="C15" t="n">
+        <v>35</v>
       </c>
       <c r="D15" t="n">
-        <v>95</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16">
@@ -1606,334 +1347,29 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Green! A room of...</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>5</v>
-      </c>
-      <c r="C17" t="n">
-        <v>7</v>
-      </c>
+          <t>#31 Silbury 2min...</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>39</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Holly Tree Hidea...</t>
+          <t>Green! A room of...</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4.92</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="D18" t="n">
-        <v>88</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>average_rating</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>number_of_ratings</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>price_per_night</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t># 2 Luxury apart...</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>4.89</v>
-      </c>
-      <c r="C2" t="n">
-        <v>53</v>
-      </c>
-      <c r="D2" t="n">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Live music fan? ...</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>4.57</v>
-      </c>
-      <c r="C3" t="n">
-        <v>7</v>
-      </c>
-      <c r="D3" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>single room clos...</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>4.87</v>
-      </c>
-      <c r="C4" t="n">
-        <v>82</v>
-      </c>
-      <c r="D4" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>#6 Milburn,CMK l...</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>A tranquil oasis...</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>4.97</v>
-      </c>
-      <c r="C6" t="n">
-        <v>714</v>
-      </c>
-      <c r="D6" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Private annexe w...</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" t="n">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Green! A room of...</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>5</v>
-      </c>
-      <c r="C8" t="n">
-        <v>7</v>
-      </c>
-      <c r="D8" t="n">
         <v>39</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Cosy Double Room...</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>4.93</v>
-      </c>
-      <c r="C9" t="n">
-        <v>15</v>
-      </c>
-      <c r="D9" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Stylish watersid...</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="C10" t="n">
-        <v>31</v>
-      </c>
-      <c r="D10" t="n">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Single Room | Sm...</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>4.95</v>
-      </c>
-      <c r="C11" t="n">
-        <v>66</v>
-      </c>
-      <c r="D11" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Lovely Home Near...</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>4.86</v>
-      </c>
-      <c r="C12" t="n">
-        <v>7</v>
-      </c>
-      <c r="D12" t="n">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>#31 Silbury 2min...</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Willen - guest s...</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>4.98</v>
-      </c>
-      <c r="C14" t="n">
-        <v>199</v>
-      </c>
-      <c r="D14" t="n">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Relax in a Brigh...</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>4.93</v>
-      </c>
-      <c r="C15" t="n">
-        <v>266</v>
-      </c>
-      <c r="D15" t="n">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Cozy Private Roo...</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Stylish Central ...</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>4.92</v>
-      </c>
-      <c r="C17" t="n">
-        <v>300</v>
-      </c>
-      <c r="D17" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Single room in q...</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="C18" t="n">
-        <v>44</v>
-      </c>
-      <c r="D18" t="n">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3791,7 +3227,7 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>

</xml_diff>